<commit_message>
Added cursor, invalidate funtion to redraw screen, timers
</commit_message>
<xml_diff>
--- a/Notes/Fonts.xlsx
+++ b/Notes/Fonts.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dev\Github\MT_Modem\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F846E6B7-C530-4F31-979C-7F7EC942C906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{613387BD-8753-4C6F-81DF-69BCE15B88CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30825" yWindow="3675" windowWidth="21600" windowHeight="11385" xr2:uid="{31BC8694-8097-4985-99F0-37A2B6B647E7}"/>
+    <workbookView xWindow="5100" yWindow="2160" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{31BC8694-8097-4985-99F0-37A2B6B647E7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Size" sheetId="1" r:id="rId1"/>
+    <sheet name="Font" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -417,8 +417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5A09DDA-464C-4C4F-90A4-B13B015A93C8}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E4A05C-6515-4C36-B8B1-32A39EA15111}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>